<commit_message>
login fonctionel avec traitement des signIn/Up
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -78,6 +78,24 @@
   </si>
   <si>
     <t>yo 2</t>
+  </si>
+  <si>
+    <t>test_ce_pseudo</t>
+  </si>
+  <si>
+    <t>bernardoo</t>
+  </si>
+  <si>
+    <t>natafa</t>
+  </si>
+  <si>
+    <t>bernard</t>
+  </si>
+  <si>
+    <t>bernardo</t>
+  </si>
+  <si>
+    <t>bernarda</t>
   </si>
 </sst>
 </file>
@@ -199,7 +217,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C2"/>
     </row>
@@ -208,7 +226,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C3"/>
     </row>

</xml_diff>

<commit_message>
fonctionel, les code a été commenté
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>bernarda</t>
+  </si>
+  <si>
+    <t>bernardghgh</t>
+  </si>
+  <si>
+    <t>bernardfhdkfh</t>
   </si>
 </sst>
 </file>
@@ -193,7 +199,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -229,6 +235,24 @@
         <v>24</v>
       </c>
       <c r="C3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
correctionde bug sur le login
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>bernardfhdkfh</t>
+  </si>
+  <si>
+    <t>jack</t>
+  </si>
+  <si>
+    <t>queen</t>
+  </si>
+  <si>
+    <t>king</t>
+  </si>
+  <si>
+    <t>carnis</t>
   </si>
 </sst>
 </file>
@@ -199,7 +211,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -253,6 +265,42 @@
         <v>26</v>
       </c>
       <c r="C5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
le client fx passe bien a l'affichage (de test) des parties si le login a réussi, mais le code est horrible
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>carnis</t>
+  </si>
+  <si>
+    <t>bernardcac</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -301,6 +304,15 @@
         <v>30</v>
       </c>
       <c r="C9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
amelioration des afichages de parties, besoin de correction d'un bug: trop de parties affiches si 2 players
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>bernardcac</t>
+  </si>
+  <si>
+    <t>wali</t>
+  </si>
+  <si>
+    <t>jimm</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -313,6 +319,24 @@
         <v>31</v>
       </c>
       <c r="C10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
ca marche niquel mais ca affiche le mauvais gagnant
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>hfdsjuhfdjs</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>Mouni</t>
+  </si>
+  <si>
+    <t>Pierrick</t>
   </si>
 </sst>
 </file>
@@ -223,7 +235,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -349,6 +361,42 @@
         <v>34</v>
       </c>
       <c r="C13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Première version fonctionnelle du memory
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Pierrick</t>
+  </si>
+  <si>
+    <t>Franck</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -397,6 +400,15 @@
         <v>38</v>
       </c>
       <c r="C17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
client fx et werveur terminés, plus qu'a faire le client android
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -141,6 +141,18 @@
   </si>
   <si>
     <t>Franck</t>
+  </si>
+  <si>
+    <t>Baptiste</t>
+  </si>
+  <si>
+    <t>raph</t>
+  </si>
+  <si>
+    <t>yass</t>
+  </si>
+  <si>
+    <t>vincent</t>
   </si>
 </sst>
 </file>
@@ -238,7 +250,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -409,6 +421,42 @@
         <v>39</v>
       </c>
       <c r="C18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
correction des classes statiques par un des singletons
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>vincent</t>
+  </si>
+  <si>
+    <t>@mickaelbaron</t>
+  </si>
+  <si>
+    <t>mikiu</t>
   </si>
 </sst>
 </file>
@@ -250,7 +256,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -457,6 +463,24 @@
         <v>43</v>
       </c>
       <c r="C22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Version finale commentée (lire le README)
</commit_message>
<xml_diff>
--- a/memoryserver/database/BDD.xlsx
+++ b/memoryserver/database/BDD.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
   <si>
     <t xml:space="preserve">idPers</t>
   </si>
@@ -159,6 +159,15 @@
   </si>
   <si>
     <t>mikiu</t>
+  </si>
+  <si>
+    <t>@yassine</t>
+  </si>
+  <si>
+    <t>pierrick</t>
+  </si>
+  <si>
+    <t>@yassine2</t>
   </si>
 </sst>
 </file>
@@ -256,7 +265,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
@@ -481,6 +490,33 @@
         <v>45</v>
       </c>
       <c r="C24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>